<commit_message>
Correct the criteria 2.18 Authentication
</commit_message>
<xml_diff>
--- a/ASVS-checklist-en.xlsx
+++ b/ASVS-checklist-en.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="992"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="992" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="385">
   <si>
     <t>Security Category</t>
   </si>
@@ -1262,6 +1262,9 @@
   </si>
   <si>
     <t>Ensure that build processes for system level languages have all security flags enabled, such as ASLR, DEP, and security checks.</t>
+  </si>
+  <si>
+    <t>Verify that information enumeration is not possible via login, password reset, or forgot account functionality.</t>
   </si>
 </sst>
 </file>
@@ -1738,11 +1741,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2106506360"/>
-        <c:axId val="2106507768"/>
+        <c:axId val="2066181128"/>
+        <c:axId val="2066184008"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="2106506360"/>
+        <c:axId val="2066181128"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1752,7 +1755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106507768"/>
+        <c:crossAx val="2066184008"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1760,7 +1763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2106507768"/>
+        <c:axId val="2066184008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1771,7 +1774,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2106506360"/>
+        <c:crossAx val="2066181128"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2152,7 +2155,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D1" activeCellId="1" sqref="A1:A17 D1:D17"/>
     </sheetView>
   </sheetViews>
@@ -4111,8 +4114,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -4317,7 +4320,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>71</v>
+        <v>384</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>

</xml_diff>

<commit_message>
Correct the typo OSCP to OCSP
</commit_message>
<xml_diff>
--- a/ASVS-checklist-en.xlsx
+++ b/ASVS-checklist-en.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="992" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="992" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -907,9 +907,6 @@
     <t>V10.14</t>
   </si>
   <si>
-    <t>Verify that proper certification revocation, such as Online Certificate Status Protocol (OSCP) Stapling, is enabled and configured.</t>
-  </si>
-  <si>
     <t>V10.15</t>
   </si>
   <si>
@@ -1265,6 +1262,9 @@
   </si>
   <si>
     <t>Verify that information enumeration is not possible via login, password reset, or forgot account functionality.</t>
+  </si>
+  <si>
+    <t>Verify that proper certification revocation, such as Online Certificate Status Protocol (OCSP) Stapling, is enabled and configured.</t>
   </si>
 </sst>
 </file>
@@ -1741,11 +1741,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2066181128"/>
-        <c:axId val="2066184008"/>
+        <c:axId val="2108343720"/>
+        <c:axId val="2108345992"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="2066181128"/>
+        <c:axId val="2108343720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1755,7 +1755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066184008"/>
+        <c:crossAx val="2108345992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1763,7 +1763,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2066184008"/>
+        <c:axId val="2108345992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1774,7 +1774,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2066181128"/>
+        <c:crossAx val="2108343720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2156,7 +2156,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="A1:A17 D1:D17"/>
+      <selection activeCell="D1" activeCellId="1" sqref="A1:F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2494,8 +2494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2685,7 +2685,7 @@
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>278</v>
+        <v>384</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -2694,13 +2694,13 @@
     </row>
     <row r="13" spans="1:7" ht="24">
       <c r="A13" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B13" s="13">
+        <v>1</v>
+      </c>
+      <c r="C13" s="24" t="s">
         <v>279</v>
-      </c>
-      <c r="B13" s="13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>280</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -2709,13 +2709,13 @@
     </row>
     <row r="14" spans="1:7" ht="24">
       <c r="A14" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="24" t="s">
         <v>281</v>
-      </c>
-      <c r="B14" s="13">
-        <v>1</v>
-      </c>
-      <c r="C14" s="24" t="s">
-        <v>282</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -2781,13 +2781,13 @@
     </row>
     <row r="2" spans="1:7" ht="24">
       <c r="A2" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>283</v>
-      </c>
-      <c r="B2" s="13">
-        <v>1</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>284</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -2796,13 +2796,13 @@
     </row>
     <row r="3" spans="1:7" ht="24">
       <c r="A3" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>285</v>
-      </c>
-      <c r="B3" s="13">
-        <v>1</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>286</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2811,13 +2811,13 @@
     </row>
     <row r="4" spans="1:7" ht="24">
       <c r="A4" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="B4" s="17">
+        <v>2</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>287</v>
-      </c>
-      <c r="B4" s="17">
-        <v>2</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>288</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2826,13 +2826,13 @@
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="A5" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>289</v>
-      </c>
-      <c r="B5" s="17">
-        <v>2</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>290</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2841,13 +2841,13 @@
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="A6" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>291</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>292</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2856,13 +2856,13 @@
     </row>
     <row r="7" spans="1:7" ht="24">
       <c r="A7" s="7" t="s">
+        <v>292</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>293</v>
-      </c>
-      <c r="B7" s="13">
-        <v>1</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>294</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2871,13 +2871,13 @@
     </row>
     <row r="8" spans="1:7" ht="24">
       <c r="A8" s="7" t="s">
+        <v>294</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>295</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>296</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -2886,13 +2886,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
+        <v>296</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>297</v>
-      </c>
-      <c r="B9" s="13">
-        <v>1</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>298</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -2958,13 +2958,13 @@
     </row>
     <row r="2" spans="1:7" ht="24">
       <c r="A2" s="7" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="B2" s="23">
         <v>3</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -2973,13 +2973,13 @@
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="7" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B3" s="23">
         <v>3</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3045,13 +3045,13 @@
     </row>
     <row r="2" spans="1:7" ht="36">
       <c r="A2" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="B2" s="17">
+        <v>2</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>303</v>
-      </c>
-      <c r="B2" s="17">
-        <v>2</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>304</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3060,13 +3060,13 @@
     </row>
     <row r="3" spans="1:7" ht="24">
       <c r="A3" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="B3" s="17">
+        <v>2</v>
+      </c>
+      <c r="C3" s="24" t="s">
         <v>305</v>
-      </c>
-      <c r="B3" s="17">
-        <v>2</v>
-      </c>
-      <c r="C3" s="24" t="s">
-        <v>306</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3132,13 +3132,13 @@
     </row>
     <row r="2" spans="1:7" ht="27">
       <c r="A2" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>307</v>
-      </c>
-      <c r="B2" s="13">
-        <v>1</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>308</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3147,13 +3147,13 @@
     </row>
     <row r="3" spans="1:7" ht="36">
       <c r="A3" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="26" t="s">
         <v>309</v>
-      </c>
-      <c r="B3" s="13">
-        <v>1</v>
-      </c>
-      <c r="C3" s="26" t="s">
-        <v>310</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3162,13 +3162,13 @@
     </row>
     <row r="4" spans="1:7" ht="24">
       <c r="A4" s="7" t="s">
+        <v>310</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="26" t="s">
         <v>311</v>
-      </c>
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="26" t="s">
-        <v>312</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3177,13 +3177,13 @@
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="A5" s="7" t="s">
+        <v>312</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>313</v>
-      </c>
-      <c r="B5" s="13">
-        <v>1</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>314</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -3192,13 +3192,13 @@
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="A6" s="7" t="s">
+        <v>314</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>315</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>316</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -3207,13 +3207,13 @@
     </row>
     <row r="7" spans="1:7" ht="24">
       <c r="A7" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="B7" s="17">
+        <v>2</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>317</v>
-      </c>
-      <c r="B7" s="17">
-        <v>2</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>318</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3222,13 +3222,13 @@
     </row>
     <row r="8" spans="1:7" ht="24">
       <c r="A8" s="7" t="s">
+        <v>318</v>
+      </c>
+      <c r="B8" s="17">
+        <v>2</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>319</v>
-      </c>
-      <c r="B8" s="17">
-        <v>2</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>320</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -3237,13 +3237,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
+        <v>320</v>
+      </c>
+      <c r="B9" s="13">
+        <v>1</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>321</v>
-      </c>
-      <c r="B9" s="13">
-        <v>1</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>322</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -3252,13 +3252,13 @@
     </row>
     <row r="10" spans="1:7" ht="24">
       <c r="A10" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>323</v>
-      </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>324</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3324,13 +3324,13 @@
     </row>
     <row r="2" spans="1:7" ht="24">
       <c r="A2" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>325</v>
-      </c>
-      <c r="B2" s="13">
-        <v>1</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>326</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3339,13 +3339,13 @@
     </row>
     <row r="3" spans="1:7" ht="24">
       <c r="A3" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>327</v>
-      </c>
-      <c r="B3" s="13">
-        <v>1</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>328</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3354,13 +3354,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>329</v>
-      </c>
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>330</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3369,13 +3369,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>331</v>
-      </c>
-      <c r="B5" s="17">
-        <v>2</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>332</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -3384,13 +3384,13 @@
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="A6" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="B6" s="17">
+        <v>2</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>333</v>
-      </c>
-      <c r="B6" s="17">
-        <v>2</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>334</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -3399,13 +3399,13 @@
     </row>
     <row r="7" spans="1:7">
       <c r="A7" s="7" t="s">
+        <v>334</v>
+      </c>
+      <c r="B7" s="17">
+        <v>2</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>335</v>
-      </c>
-      <c r="B7" s="17">
-        <v>2</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>336</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3414,13 +3414,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
+        <v>336</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>337</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>338</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -3429,13 +3429,13 @@
     </row>
     <row r="9" spans="1:7" ht="24">
       <c r="A9" s="7" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -3444,13 +3444,13 @@
     </row>
     <row r="10" spans="1:7" ht="24">
       <c r="A10" s="7" t="s">
+        <v>340</v>
+      </c>
+      <c r="B10" s="13">
+        <v>1</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>341</v>
-      </c>
-      <c r="B10" s="13">
-        <v>1</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>342</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3459,13 +3459,13 @@
     </row>
     <row r="11" spans="1:7" ht="24">
       <c r="A11" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B11" s="23">
         <v>3</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -3474,13 +3474,13 @@
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="B12" s="13">
+        <v>1</v>
+      </c>
+      <c r="C12" s="24" t="s">
         <v>345</v>
-      </c>
-      <c r="B12" s="13">
-        <v>1</v>
-      </c>
-      <c r="C12" s="24" t="s">
-        <v>346</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -3545,13 +3545,13 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" s="7" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>347</v>
-      </c>
-      <c r="B2" s="13">
-        <v>1</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>348</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3560,13 +3560,13 @@
     </row>
     <row r="3" spans="1:7" ht="24">
       <c r="A3" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="B3" s="13">
+        <v>1</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>349</v>
-      </c>
-      <c r="B3" s="13">
-        <v>1</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>350</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3575,13 +3575,13 @@
     </row>
     <row r="4" spans="1:7">
       <c r="A4" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>351</v>
-      </c>
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>352</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3590,13 +3590,13 @@
     </row>
     <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
+        <v>352</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
+      </c>
+      <c r="C5" s="27" t="s">
         <v>353</v>
-      </c>
-      <c r="B5" s="13">
-        <v>1</v>
-      </c>
-      <c r="C5" s="27" t="s">
-        <v>354</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -3605,13 +3605,13 @@
     </row>
     <row r="6" spans="1:7" ht="24">
       <c r="A6" s="7" t="s">
+        <v>354</v>
+      </c>
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>355</v>
-      </c>
-      <c r="B6" s="13">
-        <v>1</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>356</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -3620,13 +3620,13 @@
     </row>
     <row r="7" spans="1:7" ht="24">
       <c r="A7" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="B7" s="13">
+        <v>1</v>
+      </c>
+      <c r="C7" s="24" t="s">
         <v>357</v>
-      </c>
-      <c r="B7" s="13">
-        <v>1</v>
-      </c>
-      <c r="C7" s="24" t="s">
-        <v>358</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3635,13 +3635,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
+        <v>358</v>
+      </c>
+      <c r="B8" s="13">
+        <v>1</v>
+      </c>
+      <c r="C8" s="24" t="s">
         <v>359</v>
-      </c>
-      <c r="B8" s="13">
-        <v>1</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>360</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -3650,13 +3650,13 @@
     </row>
     <row r="9" spans="1:7" ht="24">
       <c r="A9" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="B9" s="17">
+        <v>2</v>
+      </c>
+      <c r="C9" s="24" t="s">
         <v>361</v>
-      </c>
-      <c r="B9" s="17">
-        <v>2</v>
-      </c>
-      <c r="C9" s="24" t="s">
-        <v>362</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -3665,13 +3665,13 @@
     </row>
     <row r="10" spans="1:7">
       <c r="A10" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B10" s="17">
+        <v>2</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>363</v>
-      </c>
-      <c r="B10" s="17">
-        <v>2</v>
-      </c>
-      <c r="C10" s="24" t="s">
-        <v>364</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3680,13 +3680,13 @@
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -3751,13 +3751,13 @@
     </row>
     <row r="2" spans="1:7" ht="36">
       <c r="A2" s="7" t="s">
+        <v>365</v>
+      </c>
+      <c r="B2" s="13">
+        <v>1</v>
+      </c>
+      <c r="C2" s="24" t="s">
         <v>366</v>
-      </c>
-      <c r="B2" s="13">
-        <v>1</v>
-      </c>
-      <c r="C2" s="24" t="s">
-        <v>367</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3766,13 +3766,13 @@
     </row>
     <row r="3" spans="1:7" ht="24">
       <c r="A3" s="7" t="s">
+        <v>367</v>
+      </c>
+      <c r="B3" s="17">
+        <v>2</v>
+      </c>
+      <c r="C3" s="25" t="s">
         <v>368</v>
-      </c>
-      <c r="B3" s="17">
-        <v>2</v>
-      </c>
-      <c r="C3" s="25" t="s">
-        <v>369</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3781,13 +3781,13 @@
     </row>
     <row r="4" spans="1:7" ht="24">
       <c r="A4" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="B4" s="17">
+        <v>2</v>
+      </c>
+      <c r="C4" s="24" t="s">
         <v>370</v>
-      </c>
-      <c r="B4" s="17">
-        <v>2</v>
-      </c>
-      <c r="C4" s="24" t="s">
-        <v>371</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3796,13 +3796,13 @@
     </row>
     <row r="5" spans="1:7" ht="24">
       <c r="A5" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2</v>
+      </c>
+      <c r="C5" s="24" t="s">
         <v>372</v>
-      </c>
-      <c r="B5" s="17">
-        <v>2</v>
-      </c>
-      <c r="C5" s="24" t="s">
-        <v>373</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -3811,13 +3811,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" s="7" t="s">
+        <v>373</v>
+      </c>
+      <c r="B6" s="17">
+        <v>2</v>
+      </c>
+      <c r="C6" s="24" t="s">
         <v>374</v>
-      </c>
-      <c r="B6" s="17">
-        <v>2</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>375</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -3826,13 +3826,13 @@
     </row>
     <row r="7" spans="1:7" ht="24">
       <c r="A7" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3841,13 +3841,13 @@
     </row>
     <row r="8" spans="1:7">
       <c r="A8" s="7" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B8" s="23">
         <v>3</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -3856,13 +3856,13 @@
     </row>
     <row r="9" spans="1:7">
       <c r="A9" s="7" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -3871,13 +3871,13 @@
     </row>
     <row r="10" spans="1:7" ht="24">
       <c r="A10" s="7" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B10" s="23">
         <v>3</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -4114,7 +4114,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
@@ -4320,7 +4320,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>

</xml_diff>

<commit_message>
Thanks to cln@scalepoint.com, i corrected excel calculation
</commit_message>
<xml_diff>
--- a/ASVS-checklist-en.xlsx
+++ b/ASVS-checklist-en.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="992" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -1679,7 +1679,7 @@
             <c:numRef>
               <c:f>'ASVS Results'!$D$2:$D$17</c:f>
               <c:numCache>
-                <c:formatCode>#,##0.00;\-#,##0.00</c:formatCode>
+                <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.0</c:v>
@@ -1741,11 +1741,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2108343720"/>
-        <c:axId val="2108345992"/>
+        <c:axId val="2115179016"/>
+        <c:axId val="2115179368"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="2108343720"/>
+        <c:axId val="2115179016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1755,7 +1755,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108345992"/>
+        <c:crossAx val="2115179368"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1763,18 +1763,18 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2108345992"/>
+        <c:axId val="2115179368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
-        <c:numFmt formatCode="#,##0.00;\-#,##0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="#,##0.00_);\(#,##0.00\)" sourceLinked="1"/>
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2108343720"/>
+        <c:crossAx val="2115179016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2155,8 +2155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D1" activeCellId="1" sqref="A1:F17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
@@ -2194,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="8">
-        <f>COUNTIF(Architecture!E2:E11,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF(Architecture!D2:D11,"&lt;&gt;Not Applicable")</f>
         <v>10</v>
       </c>
       <c r="D2" s="6">
@@ -2212,7 +2212,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="8">
-        <f>COUNTIF(Authentication!E2:E27,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF(Authentication!D2:D27,"&lt;&gt;Not Applicable")</f>
         <v>26</v>
       </c>
       <c r="D3" s="6">
@@ -2230,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="C4" s="8">
-        <f>COUNTIF('Session Management'!E2:E14,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Session Management'!D2:D14,"&lt;&gt;Not Applicable")</f>
         <v>13</v>
       </c>
       <c r="D4" s="6">
@@ -2248,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="C5" s="8">
-        <f>COUNTIF('Access Control'!E2:E13,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Access Control'!D2:D13,"&lt;&gt;Not Applicable")</f>
         <v>12</v>
       </c>
       <c r="D5" s="6">
@@ -2266,7 +2266,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="8">
-        <f>COUNTIF('Malicious Input Control'!E2:E22,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Malicious Input Control'!D2:D22,"&lt;&gt;Not Applicable")</f>
         <v>21</v>
       </c>
       <c r="D6" s="6">
@@ -2284,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="8">
-        <f>COUNTIF('Cryptography at Rest'!E2:E11,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Cryptography at Rest'!D2:D11,"&lt;&gt;Not Applicable")</f>
         <v>10</v>
       </c>
       <c r="D7" s="6">
@@ -2303,7 +2303,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="8">
-        <f>COUNTIF('Error Handling and Logging'!E2:E13,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Error Handling and Logging'!D2:D13,"&lt;&gt;Not Applicable")</f>
         <v>12</v>
       </c>
       <c r="D8" s="6">
@@ -2321,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="C9" s="8">
-        <f>COUNTIF('Data Protection'!E2:E12,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Data Protection'!D2:D12,"&lt;&gt;Not Applicable")</f>
         <v>11</v>
       </c>
       <c r="D9" s="6">
@@ -2339,7 +2339,7 @@
         <v>0</v>
       </c>
       <c r="C10" s="8">
-        <f>COUNTIF('Communication Security'!E2:E14,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Communication Security'!D2:D14,"&lt;&gt;Not Applicable")</f>
         <v>13</v>
       </c>
       <c r="D10" s="6">
@@ -2357,7 +2357,7 @@
         <v>0</v>
       </c>
       <c r="C11" s="8">
-        <f>COUNTIF('HTTP Security'!E2:E9,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('HTTP Security'!D2:D9,"&lt;&gt;Not Applicable")</f>
         <v>8</v>
       </c>
       <c r="D11" s="6">
@@ -2375,7 +2375,7 @@
         <v>0</v>
       </c>
       <c r="C12" s="8">
-        <f>COUNTIF('Malicious Control'!E2:E3,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Malicious Control'!D2:D3,"&lt;&gt;Not Applicable")</f>
         <v>2</v>
       </c>
       <c r="D12" s="6">
@@ -2393,7 +2393,7 @@
         <v>0</v>
       </c>
       <c r="C13" s="8">
-        <f>COUNTIF('Business Logic'!E2:E3,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Business Logic'!D2:D3,"&lt;&gt;Not Applicable")</f>
         <v>2</v>
       </c>
       <c r="D13" s="6">
@@ -2411,7 +2411,7 @@
         <v>0</v>
       </c>
       <c r="C14" s="8">
-        <f>COUNTIF('Files and Resources'!E2:E10,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Files and Resources'!D2:D10,"&lt;&gt;Not Applicable")</f>
         <v>9</v>
       </c>
       <c r="D14" s="6">
@@ -2429,7 +2429,7 @@
         <v>0</v>
       </c>
       <c r="C15" s="8">
-        <f>COUNTIF(Mobile!E2:E12,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF(Mobile!D2:D12,"&lt;&gt;Not Applicable")</f>
         <v>11</v>
       </c>
       <c r="D15" s="6">
@@ -2447,7 +2447,7 @@
         <v>0</v>
       </c>
       <c r="C16" s="8">
-        <f>COUNTIF('Web Services'!E2:E11,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF('Web Services'!D2:D11,"&lt;&gt;Not Applicable")</f>
         <v>10</v>
       </c>
       <c r="D16" s="6">
@@ -2465,7 +2465,7 @@
         <v>0</v>
       </c>
       <c r="C17" s="8">
-        <f>COUNTIF(Configuration!E2:E10,"&lt;&gt;Not Applicable")</f>
+        <f>COUNTIF(Configuration!D2:D10,"&lt;&gt;Not Applicable")</f>
         <v>9</v>
       </c>
       <c r="D17" s="6">
@@ -2494,7 +2494,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update to ASVS 3.0.1
</commit_message>
<xml_diff>
--- a/ASVS-checklist-en.xlsx
+++ b/ASVS-checklist-en.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e/source/github.com/emilva/owasp-asvs-checklist/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="5160" yWindow="620" windowWidth="43260" windowHeight="22900" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -25,8 +30,11 @@
     <sheet name="Web Services" sheetId="16" r:id="rId16"/>
     <sheet name="Configuration" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -35,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="394">
   <si>
     <t>Security Category</t>
   </si>
@@ -191,9 +199,6 @@
     <t>V2.2</t>
   </si>
   <si>
-    <t>Verify all password fields do not echo the user’s password when it is entered.</t>
-  </si>
-  <si>
     <t>V2.4</t>
   </si>
   <si>
@@ -209,9 +214,6 @@
     <t>V2.7</t>
   </si>
   <si>
-    <t>Verify password entry fields allow, or encourage, the use of passphrases, and do not prevent long passphrases/highly complex passwords being entered.</t>
-  </si>
-  <si>
     <t>V2.8</t>
   </si>
   <si>
@@ -227,15 +229,9 @@
     <t>V2.12</t>
   </si>
   <si>
-    <t>Verify that all suspicious authentication decisions are logged. This should include requests with relevant metadata needed for security investigations.</t>
-  </si>
-  <si>
     <t>V2.13</t>
   </si>
   <si>
-    <t>Verify that account passwords make use of a sufficient strength encryption routine and that it withstands brute force attack against the encryption routine.</t>
-  </si>
-  <si>
     <t>V2.16</t>
   </si>
   <si>
@@ -263,9 +259,6 @@
     <t>V2.20</t>
   </si>
   <si>
-    <t>Verify that request throttling is in place to prevent automated attacks against common authentication attacks such as brute force attacks or denial of service attacks.</t>
-  </si>
-  <si>
     <t>V2.21</t>
   </si>
   <si>
@@ -275,9 +268,6 @@
     <t>V2.22</t>
   </si>
   <si>
-    <t>Verify that forgotten password and other recovery paths use a soft token, mobile push, or an offline recovery mechanism.</t>
-  </si>
-  <si>
     <t>V2.23</t>
   </si>
   <si>
@@ -287,16 +277,10 @@
     <t>V2.24</t>
   </si>
   <si>
-    <t>Verify that if knowledge based questions (also known as "secret questions") are required, the questions should be strong enough to protect the application.</t>
-  </si>
-  <si>
     <t>V2.25</t>
   </si>
   <si>
     <t>V2.26</t>
-  </si>
-  <si>
-    <t>Verify re-authentication, step up or adaptive authentication, two factor authentication, or transaction signing is required before any application-specific sensitive operations are permitted as per the risk profile of the application.</t>
   </si>
   <si>
     <t>V2.27</t>
@@ -675,9 +659,6 @@
     <t>V7.11</t>
   </si>
   <si>
-    <t>Verify that all consumers of cryptographic services do not have direct access to key material. Isolate cryptographic processes, including master secrets and consider the use of a hardware key vault (HSM).</t>
-  </si>
-  <si>
     <t>V7.12</t>
   </si>
   <si>
@@ -685,9 +666,6 @@
   </si>
   <si>
     <t>V7.13</t>
-  </si>
-  <si>
-    <t>Verify that where possible, keys and secrets are zeroed when destroyed.</t>
   </si>
   <si>
     <t>V7.14</t>
@@ -940,9 +918,6 @@
     <t>V11.4</t>
   </si>
   <si>
-    <t>Verify that the Content Security Policy V2 (CSP) is in use for sites where content should not be viewed in a 3rd-party X-Frame.</t>
-  </si>
-  <si>
     <t>V11.5</t>
   </si>
   <si>
@@ -958,9 +933,6 @@
     <t>V11.7</t>
   </si>
   <si>
-    <t>Verify that the Content Security Policy V2 (CSP) is in use in a way that either disables inline JavaScript or provides an integrity check on inline JavaScript with CSP noncing or hashing.</t>
-  </si>
-  <si>
     <t>V11.8</t>
   </si>
   <si>
@@ -974,9 +946,6 @@
   </si>
   <si>
     <t>V13.2</t>
-  </si>
-  <si>
-    <t>Verify that a code review looks for malicious code, back doors, Easter eggs, and logic flaws.</t>
   </si>
   <si>
     <t>V15.1</t>
@@ -1141,15 +1110,9 @@
     <t>V17.10</t>
   </si>
   <si>
-    <t>Verify that mutable structures have been used for sensitive strings such as account numbers and are overwritten when not used. (Mitigate damage from memory analysis attacks).</t>
-  </si>
-  <si>
     <t>V17.11</t>
   </si>
   <si>
-    <t>Verify that the app’s exposed activities, intents, content providers etc. validate all inputs.</t>
-  </si>
-  <si>
     <t>V18.1</t>
   </si>
   <si>
@@ -1177,9 +1140,6 @@
     <t>V18.5</t>
   </si>
   <si>
-    <t>Verify that SOAP based web services are compliant with Web Services-Interoperability (WS-I) Basic Profile at minimum.</t>
-  </si>
-  <si>
     <t>V18.6</t>
   </si>
   <si>
@@ -1189,9 +1149,6 @@
     <t>V18.7</t>
   </si>
   <si>
-    <t>Verify that the REST service is protected from Cross-Site Request Forgery.</t>
-  </si>
-  <si>
     <t>V18.8</t>
   </si>
   <si>
@@ -1201,9 +1158,6 @@
     <t>V18.9</t>
   </si>
   <si>
-    <t>Verify that the message payload is signed to ensure reliable transport between client and service.</t>
-  </si>
-  <si>
     <t>Verify that alternative and less secure access paths do not exist.</t>
   </si>
   <si>
@@ -1265,6 +1219,91 @@
   </si>
   <si>
     <t>Verify that proper certification revocation, such as Online Certificate Status Protocol (OCSP) Stapling, is enabled and configured.</t>
+  </si>
+  <si>
+    <t>V1.11</t>
+  </si>
+  <si>
+    <t>Verify that all application components, libraries, modules,
+frameworks, platform, and operating systems are free
+from known vulnerabilities</t>
+  </si>
+  <si>
+    <t>V2.33</t>
+  </si>
+  <si>
+    <t>Browser autocomplete, and integration with password
+managers are permitted unless prohibited by risk based
+policy.</t>
+  </si>
+  <si>
+    <t>Verify that sensitive passwords or key material maintained in memory is overwritten with zeros as soon as it no longer required, to mitigate memory dumping attacks.</t>
+  </si>
+  <si>
+    <t>V8.13</t>
+  </si>
+  <si>
+    <t>Time sources should be synchronized to ensure logs have the correct time</t>
+  </si>
+  <si>
+    <t>Verify that a suitable X-FRAME-OPTIONS header is in use for sites where content should not be viewed in a 3rd-party X-Frame.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that a content security policy (CSPv2) is in place that helps mitigate common DOM, XSS, JSON, and JavaScript injection vulnerabilities. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that the application source code, and as many third party libraries as possible, does not contain back doors, Easter eggs, and logic flaws in authentication, access control, input validation, and the business logic of high value transactions. </t>
+  </si>
+  <si>
+    <t>Verify that sensitive information maintained in memory is overwritten with zeros as soon as it no longer required, to mitigate memory dumping attacks</t>
+  </si>
+  <si>
+    <t>Verify that the app validates input to exported activities, intents, or content providers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that SOAP based web services are compliant with Web Services-Interoperability (WS-I) Basic Profile at minimum. This essentially means TLS encryption. </t>
+  </si>
+  <si>
+    <t>Verify that the REST service is protected from Cross-Site Request Forgery via the use of at least one or more of the following: ORIGIN checks, double submit cookie pattern, CSRF nonces, and referrer checks.</t>
+  </si>
+  <si>
+    <t>Verify that the message payload is signed to ensure reliable transport between client and service, using JSON Web Signing or WS-Security for SOAP requests.</t>
+  </si>
+  <si>
+    <t>V18.10</t>
+  </si>
+  <si>
+    <t>V19.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that all application assets are hosted by the application, such as JavaScript libraries, CSS stylesheets and web fonts are hosted by the application rather than rely on a CDN or external provider. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that forms containing credentials are not filled in by the application. Pre-filling by the application implies that credentials are stored in plaintext or a reversible format, which is explicitly prohibited. </t>
+  </si>
+  <si>
+    <t>Verify password entry fields allow, or encourage, the use of passphrases, and do not prevent password managers, long passphrases or highly complex passwords being entered.</t>
+  </si>
+  <si>
+    <t>Verify that all authentication decisions can be logged, without storing sensitive session identifiers or passwords. This should include requests with relevant metadata needed for security investigations.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that account passwords are one way hashed with a salt, and there is sufficient work factor to defeat brute force and password hash recovery attacks. </t>
+  </si>
+  <si>
+    <t>Verify that anti-automation is in place to prevent breached credential testing, brute forcing, and account lockout attacks.</t>
+  </si>
+  <si>
+    <t>Verify that forgotten password and other recovery paths use a TOTP or other soft token, mobile push, or other offline recovery mechanism. Use of a random value in an e-mail or SMS should be a last resort and is known weak.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that if shared knowledge based questions (also known as "secret questions") are required, the questions do not violate privacy laws and are sufficiently strong to protect accounts from malicious recovery. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that risk based re-authentication, two factor or transaction signing is in place for high value transactions. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that all consumers of cryptographic services do not have direct access to key material. Isolate cryptographic processes, including master secrets and consider the use of a virtualized or physical hardware key vault (HSM). </t>
   </si>
 </sst>
 </file>
@@ -1578,6 +1617,11 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1741,21 +1785,22 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2115179016"/>
-        <c:axId val="2115179368"/>
+        <c:axId val="-928214896"/>
+        <c:axId val="-928212576"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="2115179016"/>
+        <c:axId val="-928214896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
         <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115179368"/>
+        <c:crossAx val="-928212576"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1763,7 +1808,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2115179368"/>
+        <c:axId val="-928212576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1774,7 +1819,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2115179016"/>
+        <c:crossAx val="-928214896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2155,11 +2200,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="49.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -2168,7 +2213,7 @@
     <col min="5" max="5" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="17">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2185,7 +2230,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="17">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
@@ -2203,7 +2248,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="17">
+    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2221,7 +2266,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="17">
+    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -2239,7 +2284,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="17">
+    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2257,7 +2302,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="17">
+    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2275,7 +2320,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="17">
+    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -2294,7 +2339,7 @@
       <c r="E7" s="7"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="17">
+    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
@@ -2312,7 +2357,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="17">
+    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2330,7 +2375,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="17">
+    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -2348,7 +2393,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="17">
+    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2366,7 +2411,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="17">
+    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -2384,7 +2429,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="17">
+    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -2402,7 +2447,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="17">
+    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -2420,7 +2465,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="17">
+    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -2438,7 +2483,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:6" ht="17">
+    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2456,7 +2501,7 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="17">
+    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
@@ -2482,11 +2527,6 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2495,16 +2535,16 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="88.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -2527,195 +2567,195 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24">
+    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="36">
+    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="B4" s="23">
         <v>3</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="24">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="B5" s="23">
         <v>3</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>269</v>
-      </c>
-      <c r="B8" s="23">
-        <v>3</v>
+        <v>259</v>
+      </c>
+      <c r="B8" s="17">
+        <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="B10" s="23">
         <v>3</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="24">
+    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>384</v>
+        <v>366</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="24">
+    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="24">
+    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -2734,11 +2774,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2747,16 +2782,16 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="87.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -2779,120 +2814,120 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24">
+    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="24">
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="24">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>289</v>
+        <v>374</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>290</v>
+        <v>279</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>291</v>
+        <v>280</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>292</v>
+        <v>281</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>293</v>
+        <v>282</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>294</v>
+        <v>283</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>295</v>
+        <v>375</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>296</v>
+        <v>284</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>297</v>
+        <v>285</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -2911,11 +2946,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -2924,16 +2954,16 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="88.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -2956,30 +2986,30 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24">
+    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>298</v>
+        <v>286</v>
       </c>
       <c r="B2" s="23">
         <v>3</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>299</v>
+        <v>287</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>300</v>
+        <v>288</v>
       </c>
       <c r="B3" s="23">
         <v>3</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>301</v>
+        <v>376</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2998,11 +3028,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3014,13 +3039,13 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="71.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3043,30 +3068,30 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36">
+    <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="B2" s="17">
         <v>2</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>303</v>
+        <v>290</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>304</v>
+        <v>291</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>305</v>
+        <v>292</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3085,11 +3110,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3101,13 +3121,13 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="78.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3130,135 +3150,135 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="27">
+    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>306</v>
+        <v>293</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>307</v>
+        <v>294</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="36">
+    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>308</v>
+        <v>295</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>309</v>
+        <v>296</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="24">
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>310</v>
+        <v>297</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>311</v>
+        <v>298</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="24">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>312</v>
+        <v>299</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>313</v>
+        <v>300</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>314</v>
+        <v>301</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>316</v>
+        <v>303</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>317</v>
+        <v>304</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>318</v>
+        <v>305</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>319</v>
+        <v>306</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>320</v>
+        <v>307</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>321</v>
+        <v>308</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>322</v>
+        <v>309</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>323</v>
+        <v>310</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3277,11 +3297,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3290,16 +3305,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="90" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3322,165 +3337,165 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24">
+    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>324</v>
+        <v>311</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>325</v>
+        <v>312</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>326</v>
+        <v>313</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>327</v>
+        <v>314</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>328</v>
+        <v>315</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>329</v>
+        <v>316</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>330</v>
+        <v>317</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>331</v>
+        <v>318</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>332</v>
+        <v>319</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>334</v>
+        <v>321</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>335</v>
+        <v>322</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>336</v>
+        <v>323</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>337</v>
+        <v>324</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>338</v>
+        <v>325</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>339</v>
+        <v>326</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>340</v>
+        <v>327</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>341</v>
+        <v>328</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="24">
+    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>342</v>
-      </c>
-      <c r="B11" s="23">
-        <v>3</v>
+        <v>329</v>
+      </c>
+      <c r="B11" s="17">
+        <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>343</v>
+        <v>377</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>344</v>
+        <v>330</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>345</v>
+        <v>378</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -3499,11 +3514,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -3512,15 +3522,15 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="84.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3543,150 +3553,150 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>346</v>
+        <v>331</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>347</v>
+        <v>332</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>348</v>
+        <v>333</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>351</v>
+        <v>336</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>352</v>
+        <v>337</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>353</v>
+        <v>338</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>354</v>
+        <v>339</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>355</v>
+        <v>379</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>359</v>
+        <v>380</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>361</v>
+        <v>344</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>362</v>
+        <v>345</v>
       </c>
       <c r="B10" s="17">
         <v>2</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>363</v>
+        <v>381</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>362</v>
+        <v>382</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>364</v>
+        <v>346</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -3705,28 +3715,23 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="88.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3749,140 +3754,151 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="36">
+    <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>365</v>
+        <v>347</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>366</v>
+        <v>348</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>367</v>
+        <v>349</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>368</v>
+        <v>350</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="24">
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>369</v>
+        <v>351</v>
       </c>
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>370</v>
+        <v>352</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="24">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>371</v>
+        <v>353</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>372</v>
+        <v>354</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>374</v>
+        <v>356</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>375</v>
+        <v>357</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>376</v>
+        <v>358</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>377</v>
+        <v>359</v>
       </c>
       <c r="B8" s="23">
         <v>3</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>378</v>
+        <v>360</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>379</v>
+        <v>361</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>380</v>
+        <v>362</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>381</v>
+        <v>363</v>
       </c>
       <c r="B10" s="23">
         <v>3</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>382</v>
+        <v>364</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+      <c r="A11" s="7" t="s">
+        <v>383</v>
+      </c>
+      <c r="B11" s="23">
+        <v>3</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>384</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -3896,28 +3912,23 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="63.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.5" customHeight="1">
+    <row r="1" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3940,7 +3951,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>28</v>
       </c>
@@ -3955,7 +3966,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="36">
+    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
@@ -3970,7 +3981,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
@@ -3985,7 +3996,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" ht="24">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
@@ -4000,7 +4011,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="36">
+    <row r="6" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
@@ -4015,7 +4026,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="36">
+    <row r="7" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
@@ -4030,7 +4041,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
         <v>40</v>
       </c>
@@ -4045,7 +4056,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" ht="36">
+    <row r="9" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
         <v>42</v>
       </c>
@@ -4060,7 +4071,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" ht="36">
+    <row r="10" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
         <v>44</v>
       </c>
@@ -4075,7 +4086,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" ht="24">
+    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
         <v>46</v>
       </c>
@@ -4089,6 +4100,17 @@
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A12" s="12" t="s">
+        <v>367</v>
+      </c>
+      <c r="B12" s="19">
+        <v>2</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>368</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4102,29 +4124,24 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="73" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -4147,7 +4164,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.25" customHeight="1">
+    <row r="2" spans="1:7" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="12" t="s">
         <v>48</v>
       </c>
@@ -4162,7 +4179,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>50</v>
       </c>
@@ -4170,372 +4187,383 @@
         <v>1</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>51</v>
+        <v>385</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="16"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="13">
+        <v>1</v>
+      </c>
+      <c r="C4" s="22" t="s">
         <v>52</v>
-      </c>
-      <c r="B4" s="13">
-        <v>1</v>
-      </c>
-      <c r="C4" s="22" t="s">
-        <v>53</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="16"/>
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="12" t="s">
+        <v>53</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>54</v>
-      </c>
-      <c r="B5" s="13">
-        <v>1</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>55</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="16"/>
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>57</v>
+        <v>386</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="36">
+    <row r="7" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A7" s="12" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="16"/>
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="12" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="16"/>
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A9" s="12" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>63</v>
+        <v>387</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="12" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="B10" s="17">
         <v>2</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>65</v>
+        <v>388</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" ht="24">
+    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="12" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="16"/>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" ht="24">
+    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="16"/>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" ht="24">
+    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="12" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>383</v>
+        <v>365</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" ht="24">
+    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="16"/>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="24">
+    <row r="15" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A15" s="12" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B15" s="13">
         <v>1</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>75</v>
+        <v>389</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:7" ht="24">
+    <row r="16" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A16" s="12" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B16" s="17">
         <v>2</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="16"/>
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:7" ht="24">
+    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A17" s="12" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B17" s="13">
         <v>1</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>79</v>
+        <v>390</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:7" ht="36">
+    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A18" s="12" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B18" s="17">
         <v>2</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="16"/>
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" ht="24">
+    <row r="19" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A19" s="12" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B19" s="13">
         <v>1</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>83</v>
+        <v>391</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:7" ht="24">
+    <row r="20" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" s="12" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="B20" s="17">
         <v>2</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="16"/>
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:7" ht="36">
+    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="12" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="B21" s="17">
         <v>2</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>86</v>
+        <v>392</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:7" ht="24">
+    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="12" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="B22" s="13">
         <v>1</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="16"/>
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:7" ht="24">
+    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A23" s="12" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="B23" s="23">
         <v>3</v>
       </c>
       <c r="C23" s="14" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="16"/>
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="1:7" ht="24">
+    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A24" s="12" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="B24" s="23">
         <v>3</v>
       </c>
       <c r="C24" s="14" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="D24" s="15"/>
       <c r="E24" s="16"/>
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:7" ht="24">
+    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="B25" s="13">
         <v>1</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="D25" s="15"/>
       <c r="E25" s="16"/>
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" ht="36">
+    <row r="26" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="B26" s="17">
         <v>2</v>
       </c>
       <c r="C26" s="14" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D26" s="15"/>
       <c r="E26" s="16"/>
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="B27" s="13">
         <v>1</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
+    </row>
+    <row r="28" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+      <c r="A28" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="B28" s="13">
+        <v>1</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>370</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -4549,11 +4577,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4565,13 +4588,13 @@
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -4594,195 +4617,195 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24">
+    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="24">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="B5" s="23">
         <v>3</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="36">
+    <row r="11" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="24">
+    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="24">
+    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -4801,11 +4824,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -4817,13 +4835,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="68.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -4846,180 +4864,180 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="48">
+    <row r="2" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="36">
+    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="36">
+    <row r="4" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="B8" s="23">
         <v>3</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="48">
+    <row r="11" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="36">
+    <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="24">
+    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -5038,11 +5056,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5054,13 +5067,13 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="60.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -5083,315 +5096,315 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24">
+    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="24">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="B5" s="23">
         <v>3</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="36">
+    <row r="6" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="48">
+    <row r="11" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="48">
+    <row r="12" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="48">
+    <row r="13" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="B13" s="17">
         <v>2</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="24">
+    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="B14" s="17">
         <v>2</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:7" ht="60">
+    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="B15" s="17">
         <v>2</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:7" ht="48">
+    <row r="16" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="B16" s="17">
         <v>2</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7" ht="49">
+    <row r="17" spans="1:7" ht="53" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="B17" s="17">
         <v>2</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="36">
+    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="B18" s="13">
         <v>1</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
     </row>
-    <row r="19" spans="1:7" ht="24">
+    <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="B19" s="17">
         <v>2</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="1:7" ht="24">
+    <row r="20" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="B20" s="17">
         <v>2</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="24">
+    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="B21" s="17">
         <v>2</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" ht="24">
+    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="B22" s="17">
         <v>2</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -5410,11 +5423,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5422,17 +5430,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="97.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -5455,150 +5463,150 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B5" s="23">
         <v>3</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>202</v>
+        <v>393</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>206</v>
+        <v>371</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>207</v>
+        <v>197</v>
       </c>
       <c r="B10" s="17">
         <v>2</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>208</v>
+        <v>198</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="24">
+    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="B11" s="23">
         <v>3</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>210</v>
+        <v>200</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -5617,29 +5625,24 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="80.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -5662,185 +5665,196 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="24">
+    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>211</v>
+        <v>201</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>212</v>
+        <v>202</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>213</v>
+        <v>203</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="24">
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>215</v>
+        <v>205</v>
       </c>
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="24">
+    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>217</v>
+        <v>207</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>218</v>
+        <v>208</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="B6" s="23">
         <v>3</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>221</v>
+        <v>211</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>222</v>
+        <v>212</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="36">
+    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>223</v>
+        <v>213</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B10" s="23">
         <v>3</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="24">
+    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="B12" s="23">
         <v>3</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="24">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="B13" s="23">
         <v>3</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+      <c r="A14" s="7" t="s">
+        <v>372</v>
+      </c>
+      <c r="B14" s="13">
+        <v>1</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>373</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -5854,11 +5868,6 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
 
@@ -5867,16 +5876,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="93" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="34">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -5899,165 +5908,165 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="24">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="B3" s="23">
         <v>3</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="24">
+    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="60">
+    <row r="5" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="24">
+    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="24">
+    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="24">
+    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="24">
+    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="24">
+    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="24">
+    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="24">
+    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -6076,10 +6085,5 @@
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update category and formulae
</commit_message>
<xml_diff>
--- a/ASVS-checklist-en.xlsx
+++ b/ASVS-checklist-en.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/e/source/github.com/emilva/owasp-asvs-checklist/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n3567/Documents/Personal/repository/owasp-asvs-checklist/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5160" yWindow="620" windowWidth="43260" windowHeight="22900" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-11700" yWindow="-16060" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="394">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="392">
   <si>
     <t>Security Category</t>
   </si>
@@ -299,12 +299,6 @@
   </si>
   <si>
     <t>Verify that secrets, API keys, and passwords are not included in the source code, or online source code repositories.</t>
-  </si>
-  <si>
-    <t>V2.30</t>
-  </si>
-  <si>
-    <t>Verify that if an application allows users to authenticate, they use a proven secure authentication mechanism.</t>
   </si>
   <si>
     <t>V2.31</t>
@@ -1310,7 +1304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1381,6 +1375,11 @@
       <u/>
       <sz val="10"/>
       <color theme="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="6"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1543,9 +1542,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="ハイパーリンク" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
+    <cellStyle name="表示済みのハイパーリンク" xfId="2" builtinId="9" hidden="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -1628,7 +1627,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1785,11 +1784,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-928214896"/>
-        <c:axId val="-928212576"/>
+        <c:axId val="-1361412624"/>
+        <c:axId val="-1361787184"/>
       </c:radarChart>
       <c:catAx>
-        <c:axId val="-928214896"/>
+        <c:axId val="-1361412624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1800,7 +1799,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-928212576"/>
+        <c:crossAx val="-1361787184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1808,7 +1807,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-928212576"/>
+        <c:axId val="-1361787184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1819,7 +1818,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-928214896"/>
+        <c:crossAx val="-1361412624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2200,11 +2199,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="49.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -2239,8 +2238,8 @@
         <v>0</v>
       </c>
       <c r="C2" s="8">
-        <f>COUNTIF(Architecture!D2:D11,"&lt;&gt;Not Applicable")</f>
-        <v>10</v>
+        <f>COUNTIF(Architecture!D2:D12,"&lt;&gt;Not Applicable")</f>
+        <v>11</v>
       </c>
       <c r="D2" s="6">
         <f t="shared" ref="D2:D17" si="0">(B2/C2)*100</f>
@@ -2253,7 +2252,7 @@
         <v>6</v>
       </c>
       <c r="B3" s="5">
-        <f>COUNTIF(Authentication!D2:D27,"Valid")</f>
+        <f>COUNTIF(Authentication!D2:D26,"Valid")</f>
         <v>0</v>
       </c>
       <c r="C3" s="8">
@@ -2348,8 +2347,8 @@
         <v>0</v>
       </c>
       <c r="C8" s="8">
-        <f>COUNTIF('Error Handling and Logging'!D2:D13,"&lt;&gt;Not Applicable")</f>
-        <v>12</v>
+        <f>COUNTIF('Error Handling and Logging'!D2:D14,"&lt;&gt;Not Applicable")</f>
+        <v>13</v>
       </c>
       <c r="D8" s="6">
         <f t="shared" si="0"/>
@@ -2510,8 +2509,8 @@
         <v>0</v>
       </c>
       <c r="C17" s="8">
-        <f>COUNTIF(Configuration!D2:D10,"&lt;&gt;Not Applicable")</f>
-        <v>9</v>
+        <f>COUNTIF(Configuration!D2:D11,"&lt;&gt;Not Applicable")</f>
+        <v>10</v>
       </c>
       <c r="D17" s="6">
         <f t="shared" si="0"/>
@@ -2520,6 +2519,7 @@
       <c r="E17" s="7"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
   <pageSetup paperSize="9" orientation="portrait" useFirstPageNumber="1" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <headerFooter>
@@ -2535,13 +2535,16 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="88.83203125" customWidth="1"/>
+    <col min="5" max="5" width="28.33203125" customWidth="1"/>
+    <col min="6" max="6" width="26.33203125" customWidth="1"/>
+    <col min="7" max="7" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -2569,13 +2572,13 @@
     </row>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -2584,13 +2587,13 @@
     </row>
     <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2599,13 +2602,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="B4" s="23">
         <v>3</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2614,13 +2617,13 @@
     </row>
     <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="B5" s="23">
         <v>3</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2629,13 +2632,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2644,13 +2647,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2659,13 +2662,13 @@
     </row>
     <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -2674,13 +2677,13 @@
     </row>
     <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -2689,13 +2692,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="B10" s="23">
         <v>3</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -2704,13 +2707,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -2719,13 +2722,13 @@
     </row>
     <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -2734,13 +2737,13 @@
     </row>
     <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -2749,13 +2752,13 @@
     </row>
     <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -2763,6 +2766,7 @@
       <c r="G14" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -2785,10 +2789,13 @@
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="87.5" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" customWidth="1"/>
+    <col min="6" max="6" width="25.6640625" customWidth="1"/>
+    <col min="7" max="7" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -2816,13 +2823,13 @@
     </row>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -2831,13 +2838,13 @@
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2846,13 +2853,13 @@
     </row>
     <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -2861,13 +2868,13 @@
     </row>
     <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -2876,13 +2883,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -2891,13 +2898,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -2906,13 +2913,13 @@
     </row>
     <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -2921,13 +2928,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -2935,6 +2942,7 @@
       <c r="G9" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D9">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -2957,10 +2965,13 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="88.5" customWidth="1"/>
+    <col min="5" max="5" width="35.83203125" customWidth="1"/>
+    <col min="6" max="6" width="26.1640625" customWidth="1"/>
+    <col min="7" max="7" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -2988,13 +2999,13 @@
     </row>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="B2" s="23">
         <v>3</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3003,13 +3014,13 @@
     </row>
     <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="B3" s="23">
         <v>3</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3017,6 +3028,7 @@
       <c r="G3" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D3">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -3039,10 +3051,14 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="71.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5" customWidth="1"/>
+    <col min="5" max="5" width="34.6640625" customWidth="1"/>
+    <col min="6" max="6" width="34.5" customWidth="1"/>
+    <col min="7" max="7" width="37" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -3070,13 +3086,13 @@
     </row>
     <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="B2" s="17">
         <v>2</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3085,13 +3101,13 @@
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3099,6 +3115,7 @@
       <c r="G3" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D3">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -3121,10 +3138,14 @@
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="78.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="31.5" customWidth="1"/>
+    <col min="6" max="6" width="26.83203125" customWidth="1"/>
+    <col min="7" max="7" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -3152,13 +3173,13 @@
     </row>
     <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3167,13 +3188,13 @@
     </row>
     <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3182,13 +3203,13 @@
     </row>
     <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3197,13 +3218,13 @@
     </row>
     <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -3212,13 +3233,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -3227,13 +3248,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3242,13 +3263,13 @@
     </row>
     <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -3257,13 +3278,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -3272,13 +3293,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3286,6 +3307,7 @@
       <c r="G10" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D10">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -3305,13 +3327,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="90" customWidth="1"/>
+    <col min="5" max="5" width="29.5" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
+    <col min="7" max="7" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -3339,13 +3364,13 @@
     </row>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3354,13 +3379,13 @@
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3369,13 +3394,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3384,13 +3409,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>317</v>
-      </c>
-      <c r="B5" s="17">
-        <v>2</v>
+        <v>315</v>
+      </c>
+      <c r="B5" s="13">
+        <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -3399,13 +3424,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -3414,13 +3439,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3429,13 +3454,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -3444,13 +3469,13 @@
     </row>
     <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -3459,13 +3484,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3474,13 +3499,13 @@
     </row>
     <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -3489,13 +3514,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -3503,6 +3528,7 @@
       <c r="G12" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -3522,12 +3548,15 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="84.5" customWidth="1"/>
+    <col min="5" max="5" width="35.5" customWidth="1"/>
+    <col min="6" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -3555,13 +3584,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3570,13 +3599,13 @@
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3585,13 +3614,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3600,13 +3629,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="27" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -3615,13 +3644,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -3630,13 +3659,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3645,13 +3674,13 @@
     </row>
     <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -3660,13 +3689,13 @@
     </row>
     <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -3675,13 +3704,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="B10" s="17">
         <v>2</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3690,13 +3719,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -3704,6 +3733,7 @@
       <c r="G11" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -3723,12 +3753,16 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="88.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" customWidth="1"/>
+    <col min="5" max="5" width="35.33203125" customWidth="1"/>
+    <col min="6" max="6" width="20.5" customWidth="1"/>
+    <col min="7" max="7" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -3756,13 +3790,13 @@
     </row>
     <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -3771,13 +3805,13 @@
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="25" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -3786,13 +3820,13 @@
     </row>
     <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -3801,13 +3835,13 @@
     </row>
     <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -3816,13 +3850,13 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -3831,13 +3865,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -3846,13 +3880,13 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="B8" s="23">
         <v>3</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -3861,13 +3895,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -3876,13 +3910,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B10" s="23">
         <v>3</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -3891,18 +3925,23 @@
     </row>
     <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="B11" s="23">
         <v>3</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>384</v>
-      </c>
+        <v>382</v>
+      </c>
+      <c r="D11" s="15"/>
+      <c r="E11" s="15"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D10">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3920,12 +3959,16 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="3" max="3" width="63.33203125" customWidth="1"/>
+    <col min="4" max="4" width="19.1640625" customWidth="1"/>
+    <col min="5" max="5" width="30.83203125" customWidth="1"/>
+    <col min="6" max="6" width="31.6640625" customWidth="1"/>
+    <col min="7" max="7" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -3966,7 +4009,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
@@ -4000,8 +4043,8 @@
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="B5" s="17">
-        <v>2</v>
+      <c r="B5" s="18">
+        <v>3</v>
       </c>
       <c r="C5" s="14" t="s">
         <v>35</v>
@@ -4045,8 +4088,8 @@
       <c r="A8" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="18">
-        <v>3</v>
+      <c r="B8" s="19">
+        <v>2</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>41</v>
@@ -4060,8 +4103,8 @@
       <c r="A9" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="B9" s="18">
-        <v>3</v>
+      <c r="B9" s="19">
+        <v>2</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>43</v>
@@ -4103,18 +4146,23 @@
     </row>
     <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A12" s="12" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B12" s="19">
         <v>2</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>368</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="D12" s="15"/>
+      <c r="E12" s="16"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="16"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4129,16 +4177,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G28"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="73" customWidth="1"/>
+    <col min="4" max="4" width="25.5" customWidth="1"/>
+    <col min="5" max="5" width="30.33203125" customWidth="1"/>
+    <col min="6" max="6" width="33.5" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -4187,7 +4239,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="22" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="16"/>
@@ -4232,7 +4284,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="16"/>
@@ -4277,7 +4329,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="16"/>
@@ -4292,7 +4344,7 @@
         <v>2</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="16"/>
@@ -4337,7 +4389,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="16"/>
@@ -4367,7 +4419,7 @@
         <v>1</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="16"/>
@@ -4397,7 +4449,7 @@
         <v>1</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="16"/>
@@ -4427,7 +4479,7 @@
         <v>1</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="16"/>
@@ -4457,7 +4509,7 @@
         <v>2</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="16"/>
@@ -4509,12 +4561,12 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A25" s="12" t="s">
         <v>85</v>
       </c>
-      <c r="B25" s="13">
-        <v>1</v>
+      <c r="B25" s="17">
+        <v>2</v>
       </c>
       <c r="C25" s="14" t="s">
         <v>86</v>
@@ -4524,12 +4576,12 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A26" s="12" t="s">
         <v>87</v>
       </c>
-      <c r="B26" s="17">
-        <v>2</v>
+      <c r="B26" s="13">
+        <v>1</v>
       </c>
       <c r="C26" s="14" t="s">
         <v>88</v>
@@ -4539,33 +4591,23 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A27" s="12" t="s">
-        <v>89</v>
+        <v>367</v>
       </c>
       <c r="B27" s="13">
         <v>1</v>
       </c>
       <c r="C27" s="14" t="s">
-        <v>90</v>
+        <v>368</v>
       </c>
       <c r="D27" s="15"/>
       <c r="E27" s="16"/>
       <c r="F27" s="16"/>
       <c r="G27" s="16"/>
     </row>
-    <row r="28" spans="1:7" ht="39" x14ac:dyDescent="0.15">
-      <c r="A28" s="12" t="s">
-        <v>369</v>
-      </c>
-      <c r="B28" s="13">
-        <v>1</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>370</v>
-      </c>
-    </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D27">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -4585,13 +4627,16 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
+    <col min="5" max="5" width="29" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
+    <col min="7" max="7" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -4619,13 +4664,13 @@
     </row>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -4634,13 +4679,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -4649,13 +4694,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -4664,13 +4709,13 @@
     </row>
     <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>97</v>
-      </c>
-      <c r="B5" s="23">
-        <v>3</v>
+        <v>95</v>
+      </c>
+      <c r="B5" s="17">
+        <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -4679,13 +4724,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -4694,13 +4739,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -4709,13 +4754,13 @@
     </row>
     <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -4724,13 +4769,13 @@
     </row>
     <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -4739,13 +4784,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -4754,13 +4799,13 @@
     </row>
     <row r="11" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -4769,13 +4814,13 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B12" s="13">
         <v>1</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -4784,13 +4829,13 @@
     </row>
     <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -4799,13 +4844,13 @@
     </row>
     <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -4813,6 +4858,7 @@
       <c r="G14" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -4835,10 +4881,14 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="68.6640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="5" max="5" width="32.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="7" max="7" width="42.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -4866,13 +4916,13 @@
     </row>
     <row r="2" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -4881,13 +4931,13 @@
     </row>
     <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -4896,13 +4946,13 @@
     </row>
     <row r="4" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -4911,13 +4961,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -4926,13 +4976,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -4941,13 +4991,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -4956,13 +5006,13 @@
     </row>
     <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B8" s="23">
         <v>3</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -4971,13 +5021,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -4986,13 +5036,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -5001,13 +5051,13 @@
     </row>
     <row r="11" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -5016,13 +5066,13 @@
     </row>
     <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -5031,13 +5081,13 @@
     </row>
     <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" s="13">
         <v>1</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -5045,6 +5095,7 @@
       <c r="G13" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D13">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -5063,14 +5114,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="60.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="41.33203125" customWidth="1"/>
+    <col min="6" max="6" width="35.33203125" customWidth="1"/>
+    <col min="7" max="7" width="29" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -5098,13 +5153,13 @@
     </row>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -5113,13 +5168,13 @@
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B3" s="13">
         <v>1</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -5128,13 +5183,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -5143,13 +5198,13 @@
     </row>
     <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B5" s="23">
         <v>3</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -5158,13 +5213,13 @@
     </row>
     <row r="6" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B6" s="13">
         <v>1</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -5173,13 +5228,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B7" s="13">
         <v>1</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -5188,13 +5243,13 @@
     </row>
     <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B8" s="13">
         <v>1</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -5203,13 +5258,13 @@
     </row>
     <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B9" s="13">
         <v>1</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -5218,13 +5273,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -5233,13 +5288,13 @@
     </row>
     <row r="11" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" s="13">
         <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -5248,13 +5303,13 @@
     </row>
     <row r="12" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -5263,13 +5318,13 @@
     </row>
     <row r="13" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B13" s="17">
         <v>2</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -5278,13 +5333,13 @@
     </row>
     <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B14" s="17">
         <v>2</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
@@ -5293,13 +5348,13 @@
     </row>
     <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B15" s="17">
         <v>2</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -5308,13 +5363,13 @@
     </row>
     <row r="16" spans="1:7" ht="52" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B16" s="17">
         <v>2</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
@@ -5323,13 +5378,13 @@
     </row>
     <row r="17" spans="1:7" ht="53" x14ac:dyDescent="0.15">
       <c r="A17" s="7" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="B17" s="17">
         <v>2</v>
       </c>
       <c r="C17" s="24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
@@ -5338,13 +5393,13 @@
     </row>
     <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B18" s="13">
         <v>1</v>
       </c>
       <c r="C18" s="24" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
@@ -5353,13 +5408,13 @@
     </row>
     <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B19" s="17">
         <v>2</v>
       </c>
       <c r="C19" s="24" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
@@ -5368,13 +5423,13 @@
     </row>
     <row r="20" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B20" s="17">
         <v>2</v>
       </c>
       <c r="C20" s="24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
@@ -5383,13 +5438,13 @@
     </row>
     <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B21" s="17">
         <v>2</v>
       </c>
       <c r="C21" s="24" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D21" s="15"/>
       <c r="E21" s="15"/>
@@ -5398,13 +5453,13 @@
     </row>
     <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="B22" s="17">
         <v>2</v>
       </c>
       <c r="C22" s="24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
@@ -5412,6 +5467,7 @@
       <c r="G22" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D22">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -5430,14 +5486,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="97.1640625" customWidth="1"/>
+    <col min="5" max="5" width="33.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -5465,13 +5524,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -5480,13 +5539,13 @@
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -5495,13 +5554,13 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -5510,13 +5569,13 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B5" s="23">
         <v>3</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -5525,13 +5584,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -5540,28 +5599,28 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -5570,13 +5629,13 @@
     </row>
     <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B9" s="17">
         <v>2</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -5585,13 +5644,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B10" s="17">
         <v>2</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -5600,13 +5659,13 @@
     </row>
     <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B11" s="23">
         <v>3</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -5614,6 +5673,7 @@
       <c r="G11" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
@@ -5633,13 +5693,17 @@
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="80.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.6640625" customWidth="1"/>
+    <col min="5" max="5" width="31" customWidth="1"/>
+    <col min="6" max="6" width="24" customWidth="1"/>
+    <col min="7" max="7" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -5667,13 +5731,13 @@
     </row>
     <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -5682,13 +5746,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B3" s="17">
         <v>2</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -5697,13 +5761,13 @@
     </row>
     <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B4" s="17">
         <v>2</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -5712,13 +5776,13 @@
     </row>
     <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B5" s="17">
         <v>2</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -5727,13 +5791,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="B6" s="23">
-        <v>3</v>
+        <v>207</v>
+      </c>
+      <c r="B6" s="17">
+        <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -5742,13 +5806,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B7" s="17">
         <v>2</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -5757,13 +5821,13 @@
     </row>
     <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -5772,13 +5836,13 @@
     </row>
     <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -5787,13 +5851,13 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B10" s="23">
         <v>3</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -5802,13 +5866,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="B11" s="17">
-        <v>2</v>
+        <v>217</v>
+      </c>
+      <c r="B11" s="13">
+        <v>1</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -5817,13 +5881,13 @@
     </row>
     <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B12" s="23">
         <v>3</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -5832,13 +5896,13 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A13" s="7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B13" s="23">
         <v>3</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
@@ -5847,18 +5911,23 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="B14" s="13">
         <v>1</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>373</v>
-      </c>
+        <v>371</v>
+      </c>
+      <c r="D14" s="15"/>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D13">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5879,10 +5948,13 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="93" customWidth="1"/>
+    <col min="5" max="5" width="34.5" customWidth="1"/>
+    <col min="6" max="6" width="17.5" customWidth="1"/>
+    <col min="7" max="7" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
@@ -5910,13 +5982,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A2" s="7" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="B2" s="13">
         <v>1</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15"/>
@@ -5925,13 +5997,13 @@
     </row>
     <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A3" s="7" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="B3" s="23">
         <v>3</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -5940,13 +6012,13 @@
     </row>
     <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A4" s="7" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B4" s="13">
         <v>1</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15"/>
@@ -5955,13 +6027,13 @@
     </row>
     <row r="5" spans="1:7" ht="65" x14ac:dyDescent="0.15">
       <c r="A5" s="7" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="B5" s="13">
         <v>1</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D5" s="15"/>
       <c r="E5" s="15"/>
@@ -5970,13 +6042,13 @@
     </row>
     <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A6" s="7" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="B6" s="17">
         <v>2</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
@@ -5985,13 +6057,13 @@
     </row>
     <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="B7" s="23">
         <v>3</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -6000,13 +6072,13 @@
     </row>
     <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A8" s="7" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B8" s="17">
         <v>2</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -6015,13 +6087,13 @@
     </row>
     <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="B9" s="23">
         <v>3</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15"/>
@@ -6030,13 +6102,13 @@
     </row>
     <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="B10" s="13">
         <v>1</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15"/>
@@ -6045,13 +6117,13 @@
     </row>
     <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="B11" s="17">
         <v>2</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -6060,13 +6132,13 @@
     </row>
     <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
       <c r="A12" s="7" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="B12" s="17">
         <v>2</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -6074,6 +6146,7 @@
       <c r="G12" s="15"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="12"/>
   <dataValidations count="1">
     <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>

</xml_diff>

<commit_message>
#2 Correct the formulae for categories
</commit_message>
<xml_diff>
--- a/ASVS-checklist-en.xlsx
+++ b/ASVS-checklist-en.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="28109"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10115"/>
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/n3567/Documents/Personal/repository/owasp-asvs-checklist/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A9C3160-A4DB-BF4A-87B3-87CA58303800}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-11700" yWindow="-16060" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="-12580" yWindow="-16060" windowWidth="25600" windowHeight="15460" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ASVS Results" sheetId="1" r:id="rId1"/>
@@ -30,10 +31,15 @@
     <sheet name="Web Services" sheetId="16" r:id="rId16"/>
     <sheet name="Configuration" sheetId="17" r:id="rId17"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -1303,8 +1309,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="13" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1620,12 +1626,15 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="ja-JP"/>
   <c:roundedCorners val="0"/>
@@ -1639,7 +1648,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1725,56 +1733,61 @@
                 <c:formatCode>#,##0.00_);\(#,##0.00\)</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.0</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-38E6-504E-A48F-4C7990A94E80}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1825,7 +1838,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1834,7 +1846,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageMargins b="1" l="0.75" r="0.75" t="1" header="0.5" footer="0.5"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1857,7 +1869,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2196,14 +2214,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="1" max="1" width="49.33203125" customWidth="1"/>
     <col min="2" max="2" width="23.33203125" customWidth="1"/>
@@ -2212,7 +2230,7 @@
     <col min="5" max="5" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="3" customFormat="1" ht="19">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2229,12 +2247,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" s="3" customFormat="1" ht="18">
       <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="5">
-        <f>0+COUNTIF(Architecture!D2:D11,"Valid")</f>
+        <f>0+COUNTIF(Architecture!D2:D12,"Valid")</f>
         <v>0</v>
       </c>
       <c r="C2" s="8">
@@ -2247,7 +2265,7 @@
       </c>
       <c r="E2" s="7"/>
     </row>
-    <row r="3" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="18">
       <c r="A3" s="4" t="s">
         <v>6</v>
       </c>
@@ -2265,7 +2283,7 @@
       </c>
       <c r="E3" s="7"/>
     </row>
-    <row r="4" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="18">
       <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
@@ -2283,7 +2301,7 @@
       </c>
       <c r="E4" s="7"/>
     </row>
-    <row r="5" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="18">
       <c r="A5" s="4" t="s">
         <v>8</v>
       </c>
@@ -2301,7 +2319,7 @@
       </c>
       <c r="E5" s="7"/>
     </row>
-    <row r="6" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="18">
       <c r="A6" s="4" t="s">
         <v>9</v>
       </c>
@@ -2319,7 +2337,7 @@
       </c>
       <c r="E6" s="7"/>
     </row>
-    <row r="7" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="18">
       <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
@@ -2338,12 +2356,12 @@
       <c r="E7" s="7"/>
       <c r="F7" s="9"/>
     </row>
-    <row r="8" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="18">
       <c r="A8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="8">
-        <f>COUNTIF('Error Handling and Logging'!D2:D13,"Valid")</f>
+        <f>COUNTIF('Error Handling and Logging'!D2:D14,"Valid")</f>
         <v>0</v>
       </c>
       <c r="C8" s="8">
@@ -2356,7 +2374,7 @@
       </c>
       <c r="E8" s="7"/>
     </row>
-    <row r="9" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="18">
       <c r="A9" s="4" t="s">
         <v>12</v>
       </c>
@@ -2374,7 +2392,7 @@
       </c>
       <c r="E9" s="7"/>
     </row>
-    <row r="10" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="18">
       <c r="A10" s="4" t="s">
         <v>13</v>
       </c>
@@ -2392,7 +2410,7 @@
       </c>
       <c r="E10" s="7"/>
     </row>
-    <row r="11" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="18">
       <c r="A11" s="4" t="s">
         <v>14</v>
       </c>
@@ -2410,7 +2428,7 @@
       </c>
       <c r="E11" s="7"/>
     </row>
-    <row r="12" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="18">
       <c r="A12" s="4" t="s">
         <v>15</v>
       </c>
@@ -2428,7 +2446,7 @@
       </c>
       <c r="E12" s="7"/>
     </row>
-    <row r="13" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="18">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -2446,7 +2464,7 @@
       </c>
       <c r="E13" s="7"/>
     </row>
-    <row r="14" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="18">
       <c r="A14" s="4" t="s">
         <v>17</v>
       </c>
@@ -2464,7 +2482,7 @@
       </c>
       <c r="E14" s="7"/>
     </row>
-    <row r="15" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="18">
       <c r="A15" s="4" t="s">
         <v>18</v>
       </c>
@@ -2482,7 +2500,7 @@
       </c>
       <c r="E15" s="7"/>
     </row>
-    <row r="16" spans="1:6" ht="18" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="18">
       <c r="A16" s="4" t="s">
         <v>19</v>
       </c>
@@ -2500,12 +2518,12 @@
       </c>
       <c r="E16" s="7"/>
     </row>
-    <row r="17" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="18">
       <c r="A17" s="4" t="s">
         <v>20</v>
       </c>
       <c r="B17" s="5">
-        <f>COUNTIF(Configuration!D2:D10,"Valid")</f>
+        <f>COUNTIF(Configuration!D2:D11,"Valid")</f>
         <v>0</v>
       </c>
       <c r="C17" s="8">
@@ -2531,14 +2549,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="88.83203125" customWidth="1"/>
@@ -2547,7 +2565,7 @@
     <col min="7" max="7" width="37.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -2570,7 +2588,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="28">
       <c r="A2" s="7" t="s">
         <v>245</v>
       </c>
@@ -2585,7 +2603,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="42">
       <c r="A3" s="7" t="s">
         <v>247</v>
       </c>
@@ -2600,7 +2618,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14">
       <c r="A4" s="7" t="s">
         <v>249</v>
       </c>
@@ -2615,7 +2633,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="28">
       <c r="A5" s="7" t="s">
         <v>251</v>
       </c>
@@ -2630,7 +2648,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="14">
       <c r="A6" s="7" t="s">
         <v>253</v>
       </c>
@@ -2645,7 +2663,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>255</v>
       </c>
@@ -2660,7 +2678,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>257</v>
       </c>
@@ -2675,7 +2693,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>259</v>
       </c>
@@ -2690,7 +2708,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="7" t="s">
         <v>261</v>
       </c>
@@ -2705,7 +2723,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="14">
       <c r="A11" s="7" t="s">
         <v>263</v>
       </c>
@@ -2720,7 +2738,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="28">
       <c r="A12" s="7" t="s">
         <v>265</v>
       </c>
@@ -2735,7 +2753,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="28">
       <c r="A13" s="7" t="s">
         <v>266</v>
       </c>
@@ -2750,7 +2768,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="28">
       <c r="A14" s="7" t="s">
         <v>268</v>
       </c>
@@ -2768,7 +2786,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2782,14 +2800,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="87.5" customWidth="1"/>
@@ -2798,7 +2816,7 @@
     <col min="7" max="7" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -2821,7 +2839,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="28">
       <c r="A2" s="7" t="s">
         <v>270</v>
       </c>
@@ -2836,7 +2854,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="28">
       <c r="A3" s="7" t="s">
         <v>272</v>
       </c>
@@ -2851,7 +2869,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="28">
       <c r="A4" s="7" t="s">
         <v>274</v>
       </c>
@@ -2866,7 +2884,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="28">
       <c r="A5" s="7" t="s">
         <v>276</v>
       </c>
@@ -2881,7 +2899,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>277</v>
       </c>
@@ -2896,7 +2914,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>279</v>
       </c>
@@ -2911,7 +2929,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>281</v>
       </c>
@@ -2926,7 +2944,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="14">
       <c r="A9" s="7" t="s">
         <v>282</v>
       </c>
@@ -2944,7 +2962,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D9">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D9" xr:uid="{00000000-0002-0000-0A00-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -2958,14 +2976,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="88.5" customWidth="1"/>
@@ -2974,7 +2992,7 @@
     <col min="7" max="7" width="28.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -2997,7 +3015,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="28">
       <c r="A2" s="7" t="s">
         <v>284</v>
       </c>
@@ -3012,7 +3030,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="42">
       <c r="A3" s="7" t="s">
         <v>286</v>
       </c>
@@ -3030,7 +3048,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D3">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0B00-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3044,14 +3062,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="71.33203125" customWidth="1"/>
@@ -3061,7 +3079,7 @@
     <col min="7" max="7" width="37" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3084,7 +3102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="42">
       <c r="A2" s="7" t="s">
         <v>287</v>
       </c>
@@ -3099,7 +3117,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="28">
       <c r="A3" s="7" t="s">
         <v>289</v>
       </c>
@@ -3117,7 +3135,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D3">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D3" xr:uid="{00000000-0002-0000-0C00-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3131,14 +3149,14 @@
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="78.6640625" customWidth="1"/>
@@ -3148,7 +3166,7 @@
     <col min="7" max="7" width="31.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3171,7 +3189,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="31">
       <c r="A2" s="7" t="s">
         <v>291</v>
       </c>
@@ -3186,7 +3204,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="42">
       <c r="A3" s="7" t="s">
         <v>293</v>
       </c>
@@ -3201,7 +3219,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="28">
       <c r="A4" s="7" t="s">
         <v>295</v>
       </c>
@@ -3216,7 +3234,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="28">
       <c r="A5" s="7" t="s">
         <v>297</v>
       </c>
@@ -3231,7 +3249,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>299</v>
       </c>
@@ -3246,7 +3264,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>301</v>
       </c>
@@ -3261,7 +3279,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>303</v>
       </c>
@@ -3276,7 +3294,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="14">
       <c r="A9" s="7" t="s">
         <v>305</v>
       </c>
@@ -3291,7 +3309,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="7" t="s">
         <v>307</v>
       </c>
@@ -3309,7 +3327,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D10">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D10" xr:uid="{00000000-0002-0000-0D00-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3323,14 +3341,14 @@
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="90" customWidth="1"/>
@@ -3339,7 +3357,7 @@
     <col min="7" max="7" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3362,7 +3380,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="28">
       <c r="A2" s="7" t="s">
         <v>309</v>
       </c>
@@ -3377,7 +3395,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="28">
       <c r="A3" s="7" t="s">
         <v>311</v>
       </c>
@@ -3392,7 +3410,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="28">
       <c r="A4" s="7" t="s">
         <v>313</v>
       </c>
@@ -3407,7 +3425,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14">
       <c r="A5" s="7" t="s">
         <v>315</v>
       </c>
@@ -3422,7 +3440,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>317</v>
       </c>
@@ -3437,7 +3455,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="14">
       <c r="A7" s="7" t="s">
         <v>319</v>
       </c>
@@ -3452,7 +3470,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="14">
       <c r="A8" s="7" t="s">
         <v>321</v>
       </c>
@@ -3467,7 +3485,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>323</v>
       </c>
@@ -3482,7 +3500,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="7" t="s">
         <v>325</v>
       </c>
@@ -3497,7 +3515,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="28">
       <c r="A11" s="7" t="s">
         <v>327</v>
       </c>
@@ -3512,7 +3530,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="14">
       <c r="A12" s="7" t="s">
         <v>328</v>
       </c>
@@ -3530,7 +3548,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12" xr:uid="{00000000-0002-0000-0E00-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3544,14 +3562,14 @@
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="3" max="3" width="84.5" customWidth="1"/>
     <col min="5" max="5" width="35.5" customWidth="1"/>
@@ -3559,7 +3577,7 @@
     <col min="7" max="7" width="37.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3582,7 +3600,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="14">
       <c r="A2" s="7" t="s">
         <v>329</v>
       </c>
@@ -3597,7 +3615,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="28">
       <c r="A3" s="7" t="s">
         <v>331</v>
       </c>
@@ -3612,7 +3630,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14">
       <c r="A4" s="7" t="s">
         <v>333</v>
       </c>
@@ -3627,7 +3645,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7">
       <c r="A5" s="7" t="s">
         <v>335</v>
       </c>
@@ -3642,7 +3660,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>337</v>
       </c>
@@ -3657,7 +3675,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>338</v>
       </c>
@@ -3672,7 +3690,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>340</v>
       </c>
@@ -3687,7 +3705,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>341</v>
       </c>
@@ -3702,7 +3720,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="7" t="s">
         <v>343</v>
       </c>
@@ -3717,7 +3735,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="14">
       <c r="A11" s="7" t="s">
         <v>380</v>
       </c>
@@ -3735,7 +3753,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11" xr:uid="{00000000-0002-0000-0F00-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3749,14 +3767,14 @@
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="3" max="3" width="88.6640625" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
@@ -3765,7 +3783,7 @@
     <col min="7" max="7" width="33.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3788,7 +3806,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="42">
       <c r="A2" s="7" t="s">
         <v>345</v>
       </c>
@@ -3803,7 +3821,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="28">
       <c r="A3" s="7" t="s">
         <v>347</v>
       </c>
@@ -3818,7 +3836,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="28">
       <c r="A4" s="7" t="s">
         <v>349</v>
       </c>
@@ -3833,7 +3851,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="28">
       <c r="A5" s="7" t="s">
         <v>351</v>
       </c>
@@ -3848,7 +3866,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="14">
       <c r="A6" s="7" t="s">
         <v>353</v>
       </c>
@@ -3863,7 +3881,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>355</v>
       </c>
@@ -3878,7 +3896,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="14">
       <c r="A8" s="7" t="s">
         <v>357</v>
       </c>
@@ -3893,7 +3911,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="14">
       <c r="A9" s="7" t="s">
         <v>359</v>
       </c>
@@ -3908,7 +3926,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="7" t="s">
         <v>361</v>
       </c>
@@ -3923,7 +3941,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="28">
       <c r="A11" s="7" t="s">
         <v>381</v>
       </c>
@@ -3941,7 +3959,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11" xr:uid="{00000000-0002-0000-1000-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3955,14 +3973,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="3" max="3" width="63.33203125" customWidth="1"/>
     <col min="4" max="4" width="19.1640625" customWidth="1"/>
@@ -3971,7 +3989,7 @@
     <col min="7" max="7" width="41.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" ht="27.5" customHeight="1">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -3994,7 +4012,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="14">
       <c r="A2" s="12" t="s">
         <v>28</v>
       </c>
@@ -4009,7 +4027,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="42">
       <c r="A3" s="12" t="s">
         <v>30</v>
       </c>
@@ -4024,7 +4042,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14">
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
@@ -4039,7 +4057,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="28">
       <c r="A5" s="12" t="s">
         <v>34</v>
       </c>
@@ -4054,7 +4072,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="42">
       <c r="A6" s="12" t="s">
         <v>36</v>
       </c>
@@ -4069,7 +4087,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="42">
       <c r="A7" s="12" t="s">
         <v>38</v>
       </c>
@@ -4084,7 +4102,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="12" t="s">
         <v>40</v>
       </c>
@@ -4099,7 +4117,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="42">
       <c r="A9" s="12" t="s">
         <v>42</v>
       </c>
@@ -4114,7 +4132,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="42">
       <c r="A10" s="12" t="s">
         <v>44</v>
       </c>
@@ -4129,7 +4147,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="28">
       <c r="A11" s="12" t="s">
         <v>46</v>
       </c>
@@ -4144,7 +4162,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="42">
       <c r="A12" s="12" t="s">
         <v>365</v>
       </c>
@@ -4162,7 +4180,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4176,14 +4194,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="73" customWidth="1"/>
@@ -4193,7 +4211,7 @@
     <col min="7" max="7" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -4216,7 +4234,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="25.25" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="25.25" customHeight="1">
       <c r="A2" s="12" t="s">
         <v>48</v>
       </c>
@@ -4231,7 +4249,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="42">
       <c r="A3" s="12" t="s">
         <v>50</v>
       </c>
@@ -4246,7 +4264,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14">
       <c r="A4" s="12" t="s">
         <v>51</v>
       </c>
@@ -4261,7 +4279,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14">
       <c r="A5" s="12" t="s">
         <v>53</v>
       </c>
@@ -4276,7 +4294,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="12" t="s">
         <v>55</v>
       </c>
@@ -4291,7 +4309,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="42">
       <c r="A7" s="12" t="s">
         <v>56</v>
       </c>
@@ -4306,7 +4324,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="12" t="s">
         <v>58</v>
       </c>
@@ -4321,7 +4339,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="42">
       <c r="A9" s="12" t="s">
         <v>60</v>
       </c>
@@ -4336,7 +4354,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="12" t="s">
         <v>61</v>
       </c>
@@ -4351,7 +4369,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="28">
       <c r="A11" s="12" t="s">
         <v>62</v>
       </c>
@@ -4366,7 +4384,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="28">
       <c r="A12" s="12" t="s">
         <v>64</v>
       </c>
@@ -4381,7 +4399,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="28">
       <c r="A13" s="12" t="s">
         <v>66</v>
       </c>
@@ -4396,7 +4414,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="28">
       <c r="A14" s="12" t="s">
         <v>68</v>
       </c>
@@ -4411,7 +4429,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="28">
       <c r="A15" s="12" t="s">
         <v>70</v>
       </c>
@@ -4426,7 +4444,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="28">
       <c r="A16" s="12" t="s">
         <v>71</v>
       </c>
@@ -4441,7 +4459,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="42">
       <c r="A17" s="12" t="s">
         <v>73</v>
       </c>
@@ -4456,7 +4474,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="42">
       <c r="A18" s="12" t="s">
         <v>74</v>
       </c>
@@ -4471,7 +4489,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="42">
       <c r="A19" s="12" t="s">
         <v>76</v>
       </c>
@@ -4486,7 +4504,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="28">
       <c r="A20" s="12" t="s">
         <v>77</v>
       </c>
@@ -4501,7 +4519,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="28">
       <c r="A21" s="12" t="s">
         <v>78</v>
       </c>
@@ -4516,7 +4534,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="28">
       <c r="A22" s="12" t="s">
         <v>79</v>
       </c>
@@ -4531,7 +4549,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:7" ht="28">
       <c r="A23" s="12" t="s">
         <v>81</v>
       </c>
@@ -4546,7 +4564,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:7" ht="28">
       <c r="A24" s="12" t="s">
         <v>83</v>
       </c>
@@ -4561,7 +4579,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:7" ht="42">
       <c r="A25" s="12" t="s">
         <v>85</v>
       </c>
@@ -4576,7 +4594,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:7" ht="14">
       <c r="A26" s="12" t="s">
         <v>87</v>
       </c>
@@ -4591,7 +4609,7 @@
       <c r="F26" s="16"/>
       <c r="G26" s="16"/>
     </row>
-    <row r="27" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:7" ht="42">
       <c r="A27" s="12" t="s">
         <v>367</v>
       </c>
@@ -4609,7 +4627,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D27">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D27" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4623,14 +4641,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20" customWidth="1"/>
     <col min="3" max="3" width="70" customWidth="1"/>
@@ -4639,7 +4657,7 @@
     <col min="7" max="7" width="42.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -4662,7 +4680,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="28">
       <c r="A2" s="7" t="s">
         <v>89</v>
       </c>
@@ -4677,7 +4695,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="14">
       <c r="A3" s="7" t="s">
         <v>91</v>
       </c>
@@ -4692,7 +4710,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14">
       <c r="A4" s="7" t="s">
         <v>93</v>
       </c>
@@ -4707,7 +4725,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="28">
       <c r="A5" s="7" t="s">
         <v>95</v>
       </c>
@@ -4722,7 +4740,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>97</v>
       </c>
@@ -4737,7 +4755,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>99</v>
       </c>
@@ -4752,7 +4770,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>101</v>
       </c>
@@ -4767,7 +4785,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>103</v>
       </c>
@@ -4782,7 +4800,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="7" t="s">
         <v>105</v>
       </c>
@@ -4797,7 +4815,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="42">
       <c r="A11" s="7" t="s">
         <v>107</v>
       </c>
@@ -4812,7 +4830,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="14">
       <c r="A12" s="7" t="s">
         <v>109</v>
       </c>
@@ -4827,7 +4845,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="28">
       <c r="A13" s="7" t="s">
         <v>111</v>
       </c>
@@ -4842,7 +4860,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="28">
       <c r="A14" s="7" t="s">
         <v>113</v>
       </c>
@@ -4860,7 +4878,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -4874,14 +4892,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="68.6640625" customWidth="1"/>
@@ -4891,7 +4909,7 @@
     <col min="7" max="7" width="42.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -4914,7 +4932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="56">
       <c r="A2" s="7" t="s">
         <v>115</v>
       </c>
@@ -4929,7 +4947,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="42">
       <c r="A3" s="7" t="s">
         <v>117</v>
       </c>
@@ -4944,7 +4962,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="42">
       <c r="A4" s="7" t="s">
         <v>119</v>
       </c>
@@ -4959,7 +4977,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14">
       <c r="A5" s="7" t="s">
         <v>121</v>
       </c>
@@ -4974,7 +4992,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>123</v>
       </c>
@@ -4989,7 +5007,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>125</v>
       </c>
@@ -5004,7 +5022,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>127</v>
       </c>
@@ -5019,7 +5037,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>129</v>
       </c>
@@ -5034,7 +5052,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="7" t="s">
         <v>131</v>
       </c>
@@ -5049,7 +5067,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="56">
       <c r="A11" s="7" t="s">
         <v>133</v>
       </c>
@@ -5064,7 +5082,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="42">
       <c r="A12" s="7" t="s">
         <v>135</v>
       </c>
@@ -5079,7 +5097,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="28">
       <c r="A13" s="7" t="s">
         <v>137</v>
       </c>
@@ -5097,7 +5115,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D13">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D13" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5111,14 +5129,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="60.6640625" customWidth="1"/>
@@ -5128,7 +5146,7 @@
     <col min="7" max="7" width="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -5151,7 +5169,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="28">
       <c r="A2" s="7" t="s">
         <v>139</v>
       </c>
@@ -5166,7 +5184,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="28">
       <c r="A3" s="7" t="s">
         <v>141</v>
       </c>
@@ -5181,7 +5199,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="14">
       <c r="A4" s="7" t="s">
         <v>143</v>
       </c>
@@ -5196,7 +5214,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="28">
       <c r="A5" s="7" t="s">
         <v>145</v>
       </c>
@@ -5211,7 +5229,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="42">
       <c r="A6" s="7" t="s">
         <v>147</v>
       </c>
@@ -5226,7 +5244,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>149</v>
       </c>
@@ -5241,7 +5259,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>151</v>
       </c>
@@ -5256,7 +5274,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>153</v>
       </c>
@@ -5271,7 +5289,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="42">
       <c r="A10" s="7" t="s">
         <v>155</v>
       </c>
@@ -5286,7 +5304,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="56">
       <c r="A11" s="7" t="s">
         <v>157</v>
       </c>
@@ -5301,7 +5319,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="70">
       <c r="A12" s="7" t="s">
         <v>159</v>
       </c>
@@ -5316,7 +5334,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="56">
       <c r="A13" s="7" t="s">
         <v>161</v>
       </c>
@@ -5331,7 +5349,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="28">
       <c r="A14" s="7" t="s">
         <v>163</v>
       </c>
@@ -5346,7 +5364,7 @@
       <c r="F14" s="15"/>
       <c r="G14" s="15"/>
     </row>
-    <row r="15" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:7" ht="70">
       <c r="A15" s="7" t="s">
         <v>165</v>
       </c>
@@ -5361,7 +5379,7 @@
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
     </row>
-    <row r="16" spans="1:7" ht="52" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:7" ht="56">
       <c r="A16" s="7" t="s">
         <v>167</v>
       </c>
@@ -5376,7 +5394,7 @@
       <c r="F16" s="15"/>
       <c r="G16" s="15"/>
     </row>
-    <row r="17" spans="1:7" ht="53" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:7" ht="57">
       <c r="A17" s="7" t="s">
         <v>169</v>
       </c>
@@ -5391,7 +5409,7 @@
       <c r="F17" s="15"/>
       <c r="G17" s="15"/>
     </row>
-    <row r="18" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:7" ht="42">
       <c r="A18" s="7" t="s">
         <v>171</v>
       </c>
@@ -5406,7 +5424,7 @@
       <c r="F18" s="15"/>
       <c r="G18" s="15"/>
     </row>
-    <row r="19" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:7" ht="28">
       <c r="A19" s="7" t="s">
         <v>173</v>
       </c>
@@ -5421,7 +5439,7 @@
       <c r="F19" s="15"/>
       <c r="G19" s="15"/>
     </row>
-    <row r="20" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:7" ht="42">
       <c r="A20" s="7" t="s">
         <v>175</v>
       </c>
@@ -5436,7 +5454,7 @@
       <c r="F20" s="15"/>
       <c r="G20" s="15"/>
     </row>
-    <row r="21" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:7" ht="28">
       <c r="A21" s="7" t="s">
         <v>177</v>
       </c>
@@ -5451,7 +5469,7 @@
       <c r="F21" s="15"/>
       <c r="G21" s="15"/>
     </row>
-    <row r="22" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:7" ht="28">
       <c r="A22" s="7" t="s">
         <v>179</v>
       </c>
@@ -5469,7 +5487,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D22">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D22" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5483,14 +5501,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="97.1640625" customWidth="1"/>
@@ -5499,7 +5517,7 @@
     <col min="7" max="7" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -5522,7 +5540,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="14">
       <c r="A2" s="7" t="s">
         <v>181</v>
       </c>
@@ -5537,7 +5555,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="42">
       <c r="A3" s="7" t="s">
         <v>183</v>
       </c>
@@ -5552,7 +5570,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="28">
       <c r="A4" s="7" t="s">
         <v>185</v>
       </c>
@@ -5567,7 +5585,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="14">
       <c r="A5" s="7" t="s">
         <v>187</v>
       </c>
@@ -5582,7 +5600,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>189</v>
       </c>
@@ -5597,7 +5615,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>191</v>
       </c>
@@ -5612,7 +5630,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>192</v>
       </c>
@@ -5627,7 +5645,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>194</v>
       </c>
@@ -5642,7 +5660,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="14">
       <c r="A10" s="7" t="s">
         <v>195</v>
       </c>
@@ -5657,7 +5675,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="28">
       <c r="A11" s="7" t="s">
         <v>197</v>
       </c>
@@ -5675,7 +5693,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D11" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5689,14 +5707,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="80.33203125" customWidth="1"/>
@@ -5706,7 +5724,7 @@
     <col min="7" max="7" width="35.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -5729,7 +5747,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="42">
       <c r="A2" s="7" t="s">
         <v>199</v>
       </c>
@@ -5744,7 +5762,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="14">
       <c r="A3" s="7" t="s">
         <v>201</v>
       </c>
@@ -5759,7 +5777,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="28">
       <c r="A4" s="7" t="s">
         <v>203</v>
       </c>
@@ -5774,7 +5792,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="28">
       <c r="A5" s="7" t="s">
         <v>205</v>
       </c>
@@ -5789,7 +5807,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>207</v>
       </c>
@@ -5804,7 +5822,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="14">
       <c r="A7" s="7" t="s">
         <v>209</v>
       </c>
@@ -5819,7 +5837,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="39" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="56">
       <c r="A8" s="7" t="s">
         <v>211</v>
       </c>
@@ -5834,7 +5852,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>213</v>
       </c>
@@ -5849,7 +5867,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="14">
       <c r="A10" s="7" t="s">
         <v>215</v>
       </c>
@@ -5864,7 +5882,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="14">
       <c r="A11" s="7" t="s">
         <v>217</v>
       </c>
@@ -5879,7 +5897,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="28">
       <c r="A12" s="7" t="s">
         <v>219</v>
       </c>
@@ -5894,7 +5912,7 @@
       <c r="F12" s="15"/>
       <c r="G12" s="15"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:7" ht="28">
       <c r="A13" s="7" t="s">
         <v>221</v>
       </c>
@@ -5909,7 +5927,7 @@
       <c r="F13" s="15"/>
       <c r="G13" s="15"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:7" ht="14">
       <c r="A14" s="7" t="s">
         <v>370</v>
       </c>
@@ -5927,7 +5945,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D14" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -5941,14 +5959,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="12" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="20"/>
     <col min="3" max="3" width="93" customWidth="1"/>
@@ -5957,7 +5975,7 @@
     <col min="7" max="7" width="30.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="21" customFormat="1" ht="36" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:7" s="21" customFormat="1" ht="38">
       <c r="A1" s="10" t="s">
         <v>21</v>
       </c>
@@ -5980,7 +5998,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:7" ht="14">
       <c r="A2" s="7" t="s">
         <v>223</v>
       </c>
@@ -5995,7 +6013,7 @@
       <c r="F2" s="15"/>
       <c r="G2" s="15"/>
     </row>
-    <row r="3" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:7" ht="28">
       <c r="A3" s="7" t="s">
         <v>225</v>
       </c>
@@ -6010,7 +6028,7 @@
       <c r="F3" s="15"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:7" ht="28">
       <c r="A4" s="7" t="s">
         <v>227</v>
       </c>
@@ -6025,7 +6043,7 @@
       <c r="F4" s="15"/>
       <c r="G4" s="15"/>
     </row>
-    <row r="5" spans="1:7" ht="65" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:7" ht="70">
       <c r="A5" s="7" t="s">
         <v>229</v>
       </c>
@@ -6040,7 +6058,7 @@
       <c r="F5" s="15"/>
       <c r="G5" s="15"/>
     </row>
-    <row r="6" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:7" ht="28">
       <c r="A6" s="7" t="s">
         <v>231</v>
       </c>
@@ -6055,7 +6073,7 @@
       <c r="F6" s="15"/>
       <c r="G6" s="15"/>
     </row>
-    <row r="7" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:7" ht="28">
       <c r="A7" s="7" t="s">
         <v>233</v>
       </c>
@@ -6070,7 +6088,7 @@
       <c r="F7" s="15"/>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:7" ht="28">
       <c r="A8" s="7" t="s">
         <v>235</v>
       </c>
@@ -6085,7 +6103,7 @@
       <c r="F8" s="15"/>
       <c r="G8" s="15"/>
     </row>
-    <row r="9" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:7" ht="28">
       <c r="A9" s="7" t="s">
         <v>237</v>
       </c>
@@ -6100,7 +6118,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="15"/>
     </row>
-    <row r="10" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:7" ht="28">
       <c r="A10" s="7" t="s">
         <v>239</v>
       </c>
@@ -6115,7 +6133,7 @@
       <c r="F10" s="15"/>
       <c r="G10" s="15"/>
     </row>
-    <row r="11" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:7" ht="28">
       <c r="A11" s="7" t="s">
         <v>241</v>
       </c>
@@ -6130,7 +6148,7 @@
       <c r="F11" s="15"/>
       <c r="G11" s="15"/>
     </row>
-    <row r="12" spans="1:7" ht="26" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:7" ht="28">
       <c r="A12" s="7" t="s">
         <v>243</v>
       </c>
@@ -6148,7 +6166,7 @@
   </sheetData>
   <phoneticPr fontId="12"/>
   <dataValidations count="1">
-    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12">
+    <dataValidation type="list" operator="equal" showErrorMessage="1" sqref="D2:D12" xr:uid="{00000000-0002-0000-0800-000000000000}">
       <formula1>"Valid,Non-valid,Not Applicable"</formula1>
       <formula2>0</formula2>
     </dataValidation>

</xml_diff>